<commit_message>
Rspec for missing entry
</commit_message>
<xml_diff>
--- a/spec/fixtures/StatisticsReport.xlsx
+++ b/spec/fixtures/StatisticsReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuchengjiang/Downloads/606project/FPR-Extraction-Metrics/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02117EB7-31B6-684A-B297-3FDA9DA39FCA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8C0230-0BFA-C54E-A014-E1D7D2CAE720}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16700" tabRatio="460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" tabRatio="460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015CDeptStatisticsReport (1)" sheetId="1" r:id="rId1"/>
@@ -563,7 +563,7 @@
   <dimension ref="A1:AY10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -959,9 +959,7 @@
       <c r="K3" s="1">
         <v>0.9</v>
       </c>
-      <c r="L3" s="1">
-        <v>4.07</v>
-      </c>
+      <c r="L3" s="1"/>
       <c r="M3" s="1">
         <v>0.79900000000000004</v>
       </c>

</xml_diff>